<commit_message>
Updating document, after Github was cleaned up by Jamie Warner.
</commit_message>
<xml_diff>
--- a/AutomatedTest/Sections/AutomatedTestToolComparison.xlsx
+++ b/AutomatedTest/Sections/AutomatedTestToolComparison.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Tool</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>Image Capture and Scan</t>
-  </si>
-  <si>
-    <t>Optical Character Recognition</t>
   </si>
   <si>
     <t>ATRT 
@@ -127,10 +124,25 @@
     <t>Test Execution Reporting Capabilities</t>
   </si>
   <si>
-    <t>5hrs 45mins</t>
-  </si>
-  <si>
-    <t>4 hours</t>
+    <t>4 hours for success and failure scenarios</t>
+  </si>
+  <si>
+    <t>5hrs 45mins for success and failure scenarios</t>
+  </si>
+  <si>
+    <t>6hrs 30mins for success scenario only.  Failure scenario not finished</t>
+  </si>
+  <si>
+    <t>Success: 55 secs
+Failure: 40 secs</t>
+  </si>
+  <si>
+    <t>Success: 2 min 20 sec
+Failure: 1 min 20 sec</t>
+  </si>
+  <si>
+    <t>Success: 2 min 45 sec
+Failure: NOT TESTED due to management decision</t>
   </si>
 </sst>
 </file>
@@ -731,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S10"/>
+  <dimension ref="A2:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,42 +756,41 @@
     <col min="5" max="5" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="12.5703125" style="2" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="2" customWidth="1"/>
     <col min="10" max="10" width="16.85546875" style="21" customWidth="1"/>
     <col min="11" max="11" width="16.85546875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="18.42578125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="17.5703125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="13" style="2" customWidth="1"/>
-    <col min="18" max="18" width="16" style="2" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" style="2" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="2"/>
+    <col min="12" max="12" width="13.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="13" style="2" customWidth="1"/>
+    <col min="17" max="17" width="16" style="2" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" style="2" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="J2" s="18"/>
     </row>
-    <row r="3" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="18"/>
     </row>
-    <row r="4" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="J4" s="19"/>
     </row>
-    <row r="5" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="J5" s="19"/>
     </row>
-    <row r="6" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="28" t="s">
         <v>16</v>
       </c>
@@ -793,22 +804,8 @@
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
       <c r="J6" s="17"/>
-      <c r="L6" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="R6" s="24"/>
-      <c r="S6" s="25"/>
-    </row>
-    <row r="7" spans="1:19" s="1" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:18" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -837,37 +834,10 @@
         <v>20</v>
       </c>
       <c r="J7" s="17"/>
-      <c r="K7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L7" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="M7" s="14" t="s">
+    </row>
+    <row r="8" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>27</v>
-      </c>
-      <c r="N7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q7" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="R7" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="S7" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>28</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>14</v>
@@ -890,38 +860,17 @@
       <c r="H8" s="12">
         <v>6</v>
       </c>
-      <c r="I8" s="12"/>
+      <c r="I8" s="12" t="s">
+        <v>36</v>
+      </c>
       <c r="J8" s="20"/>
-      <c r="K8" s="16" t="s">
+    </row>
+    <row r="9" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="L8" s="15">
-        <v>8</v>
-      </c>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="13">
-        <v>4</v>
-      </c>
-      <c r="P8" s="13">
-        <v>3</v>
-      </c>
-      <c r="Q8" s="10">
-        <v>8</v>
-      </c>
-      <c r="R8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="S8" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>29</v>
-      </c>
       <c r="B9" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="11">
         <v>9</v>
@@ -939,39 +888,16 @@
         <v>8</v>
       </c>
       <c r="H9" s="12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J9" s="20"/>
-      <c r="K9" s="16" t="s">
+    </row>
+    <row r="10" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>29</v>
-      </c>
-      <c r="L9" s="15">
-        <v>8</v>
-      </c>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="13">
-        <v>7</v>
-      </c>
-      <c r="P9" s="13">
-        <v>8</v>
-      </c>
-      <c r="Q9" s="10">
-        <v>7</v>
-      </c>
-      <c r="R9" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="S9" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>30</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>15</v>
@@ -998,36 +924,132 @@
         <v>35</v>
       </c>
       <c r="J10" s="20"/>
-      <c r="K10" s="16" t="s">
+    </row>
+    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L13" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="27"/>
+      <c r="N13" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O13" s="22"/>
+      <c r="P13" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="25"/>
+    </row>
+    <row r="14" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+      <c r="K14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="R14" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="K15" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="15">
+        <v>8</v>
+      </c>
+      <c r="M15" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="N15" s="13">
+        <v>4</v>
+      </c>
+      <c r="O15" s="13">
+        <v>3</v>
+      </c>
+      <c r="P15" s="10">
+        <v>8</v>
+      </c>
+      <c r="Q15" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="R15" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="K16" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="L16" s="15">
+        <v>8</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="N16" s="13">
+        <v>7</v>
+      </c>
+      <c r="O16" s="13">
+        <v>8</v>
+      </c>
+      <c r="P16" s="10">
+        <v>7</v>
+      </c>
+      <c r="Q16" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="R16" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="11:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="K17" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L17" s="15">
+        <v>8</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="N17" s="13">
+        <v>7</v>
+      </c>
+      <c r="O17" s="13">
+        <v>8</v>
+      </c>
+      <c r="P17" s="10">
+        <v>7</v>
+      </c>
+      <c r="Q17" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="R17" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="L10" s="15">
-        <v>8</v>
-      </c>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="13">
-        <v>7</v>
-      </c>
-      <c r="P10" s="13">
-        <v>8</v>
-      </c>
-      <c r="Q10" s="10">
-        <v>7</v>
-      </c>
-      <c r="R10" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="S10" s="10" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:R13"/>
     <mergeCell ref="E6:I6"/>
-    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L13:M13"/>
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modified document sections and combined sections into one document.
</commit_message>
<xml_diff>
--- a/AutomatedTest/Sections/AutomatedTestToolComparison.xlsx
+++ b/AutomatedTest/Sections/AutomatedTestToolComparison.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
   <si>
     <t>Tool</t>
   </si>
@@ -143,6 +143,58 @@
   <si>
     <t>Success: 2 min 45 sec
 Failure: NOT TESTED due to management decision</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Host</t>
+  </si>
+  <si>
+    <t>SUT</t>
+  </si>
+  <si>
+    <t>License/Cost</t>
+  </si>
+  <si>
+    <t>Any that support VNC</t>
+  </si>
+  <si>
+    <t>Graphical Flowchart</t>
+  </si>
+  <si>
+    <t>Scripting (SenseTalk)</t>
+  </si>
+  <si>
+    <t>Scripting (Python)</t>
+  </si>
+  <si>
+    <t>ATRT 5.6.8</t>
+  </si>
+  <si>
+    <t>Commercial (see Appendix A)</t>
+  </si>
+  <si>
+    <t>Linux, Mac OS X, Windows</t>
+  </si>
+  <si>
+    <t>Innovative Defense Technologies idtus.com</t>
+  </si>
+  <si>
+    <t>Eggplant Functional 14.0.1</t>
+  </si>
+  <si>
+    <t>TestPlant testplant.com</t>
+  </si>
+  <si>
+    <t>Sikuli Script sikuli.org</t>
+  </si>
+  <si>
+    <t>Open Source MIT License Free</t>
+  </si>
+  <si>
+    <t>Sikuli 
+1.01</t>
   </si>
 </sst>
 </file>
@@ -336,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -426,6 +478,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -436,16 +494,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFD07876"/>
+      <color rgb="FFEBC8C7"/>
       <color rgb="FFFEF1E6"/>
       <color rgb="FFFDE6D3"/>
-      <color rgb="FFEBC8C7"/>
       <color rgb="FFBCD3EE"/>
       <color rgb="FFCDE8EF"/>
       <color rgb="FFE0DCCA"/>
       <color rgb="FFD1CBAF"/>
       <color rgb="FFC4BD97"/>
       <color rgb="FF97BAE5"/>
-      <color rgb="FF6B9EDB"/>
     </mruColors>
   </colors>
   <extLst>
@@ -743,17 +801,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R17"/>
+  <dimension ref="A2:Y24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="N13" workbookViewId="0">
+      <selection activeCell="T21" sqref="T21:Y24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" style="2" customWidth="1"/>
     <col min="2" max="4" width="12.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="2" customWidth="1"/>
     <col min="6" max="7" width="12.5703125" style="2" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" style="2" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" style="2" customWidth="1"/>
@@ -766,7 +824,14 @@
     <col min="16" max="16" width="13" style="2" customWidth="1"/>
     <col min="17" max="17" width="16" style="2" customWidth="1"/>
     <col min="18" max="18" width="13.7109375" style="2" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="2"/>
+    <col min="19" max="19" width="9.140625" style="2"/>
+    <col min="20" max="20" width="11.7109375" style="2" customWidth="1"/>
+    <col min="21" max="21" width="16.5703125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="10" style="2" customWidth="1"/>
+    <col min="23" max="23" width="11.5703125" style="2" customWidth="1"/>
+    <col min="24" max="24" width="12.7109375" style="2" customWidth="1"/>
+    <col min="25" max="25" width="15.7109375" style="2" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1018,7 +1083,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="11:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="11:25" ht="30" x14ac:dyDescent="0.25">
       <c r="K17" s="16" t="s">
         <v>29</v>
       </c>
@@ -1042,6 +1107,86 @@
       </c>
       <c r="R17" s="10" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="11:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="T21" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="U21" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="V21" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="W21" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="X21" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y21" s="32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="11:25" ht="60" x14ac:dyDescent="0.25">
+      <c r="T22" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="U22" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="V22" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="W22" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="X22" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y22" s="31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="11:25" ht="45" x14ac:dyDescent="0.25">
+      <c r="T23" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="U23" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="V23" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="W23" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="X23" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y23" s="31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="11:25" ht="45" x14ac:dyDescent="0.25">
+      <c r="T24" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="U24" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="V24" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="W24" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="X24" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y24" s="31" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made many changes to final document and deleted intermediate files.
</commit_message>
<xml_diff>
--- a/AutomatedTest/Sections/AutomatedTestToolComparison.xlsx
+++ b/AutomatedTest/Sections/AutomatedTestToolComparison.xlsx
@@ -480,10 +480,10 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -494,6 +494,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF6B9EDB"/>
       <color rgb="FFD07876"/>
       <color rgb="FFEBC8C7"/>
       <color rgb="FFFEF1E6"/>
@@ -503,7 +504,6 @@
       <color rgb="FFE0DCCA"/>
       <color rgb="FFD1CBAF"/>
       <color rgb="FFC4BD97"/>
-      <color rgb="FF97BAE5"/>
     </mruColors>
   </colors>
   <extLst>
@@ -803,7 +803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="T21" sqref="T21:Y24"/>
     </sheetView>
   </sheetViews>
@@ -1109,83 +1109,83 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="11:25" ht="30" x14ac:dyDescent="0.25">
-      <c r="T21" s="32" t="s">
+    <row r="21" spans="11:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T21" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="U21" s="32" t="s">
+      <c r="U21" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="V21" s="32" t="s">
+      <c r="V21" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="W21" s="32" t="s">
+      <c r="W21" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="X21" s="32" t="s">
+      <c r="X21" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="Y21" s="32" t="s">
+      <c r="Y21" s="31" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="22" spans="11:25" ht="60" x14ac:dyDescent="0.25">
-      <c r="T22" s="31" t="s">
+      <c r="T22" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="U22" s="31" t="s">
+      <c r="U22" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="V22" s="31" t="s">
+      <c r="V22" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="W22" s="31" t="s">
+      <c r="W22" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="X22" s="31" t="s">
+      <c r="X22" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="Y22" s="31" t="s">
+      <c r="Y22" s="32" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" spans="11:25" ht="45" x14ac:dyDescent="0.25">
-      <c r="T23" s="31" t="s">
+      <c r="T23" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="U23" s="31" t="s">
+      <c r="U23" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="V23" s="31" t="s">
+      <c r="V23" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="W23" s="31" t="s">
+      <c r="W23" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="X23" s="31" t="s">
+      <c r="X23" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="Y23" s="31" t="s">
+      <c r="Y23" s="32" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="24" spans="11:25" ht="45" x14ac:dyDescent="0.25">
-      <c r="T24" s="31" t="s">
+      <c r="T24" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="U24" s="31" t="s">
+      <c r="U24" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="V24" s="31" t="s">
+      <c r="V24" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="W24" s="31" t="s">
+      <c r="W24" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="X24" s="31" t="s">
+      <c r="X24" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="Y24" s="31" t="s">
+      <c r="Y24" s="32" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>